<commit_message>
Edit real picture. Works better than signature.
</commit_message>
<xml_diff>
--- a/PictureEditing.xlsx
+++ b/PictureEditing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7974918A-582E-4CC4-BA47-3942D765BC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A615271-F491-420C-A798-DA17FFA202F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{490EC28C-C6AE-42AE-A8B1-5CAC9CB6998D}"/>
   </bookViews>
@@ -217,6 +217,92 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>315686</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>65315</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>52030</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Mother kissing baby girl">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C28E91D-4E17-FC69-3A53-739BBF41D92E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a14:imgLayer r:embed="rId4">
+                  <a14:imgEffect>
+                    <a14:backgroundRemoval t="9938" b="99148" l="9955" r="89970">
+                      <a14:foregroundMark x1="75776" y1="44463" x2="61204" y2="58319"/>
+                      <a14:foregroundMark x1="61204" y1="58319" x2="60371" y2="68995"/>
+                      <a14:foregroundMark x1="60371" y1="68995" x2="71385" y2="82453"/>
+                      <a14:foregroundMark x1="71385" y1="82453" x2="80507" y2="61102"/>
+                      <a14:foregroundMark x1="80507" y1="61102" x2="79296" y2="49517"/>
+                      <a14:foregroundMark x1="79296" y1="49517" x2="75776" y2="45088"/>
+                      <a14:foregroundMark x1="82210" y1="82794" x2="81075" y2="97274"/>
+                      <a14:foregroundMark x1="81075" y1="97274" x2="64232" y2="98240"/>
+                      <a14:foregroundMark x1="64232" y1="98240" x2="58592" y2="91539"/>
+                      <a14:foregroundMark x1="58592" y1="91539" x2="56548" y2="81317"/>
+                      <a14:foregroundMark x1="56548" y1="81317" x2="68055" y2="81942"/>
+                      <a14:foregroundMark x1="68055" y1="81942" x2="75814" y2="81034"/>
+                      <a14:foregroundMark x1="75814" y1="81034" x2="82362" y2="84895"/>
+                      <a14:foregroundMark x1="63172" y1="84441" x2="63172" y2="84441"/>
+                      <a14:foregroundMark x1="62036" y1="56218" x2="54921" y2="56843"/>
+                      <a14:foregroundMark x1="54921" y1="56843" x2="61090" y2="60931"/>
+                      <a14:foregroundMark x1="61090" y1="60931" x2="60636" y2="54117"/>
+                      <a14:foregroundMark x1="63588" y1="81715" x2="76684" y2="82340"/>
+                      <a14:foregroundMark x1="76684" y1="82340" x2="84595" y2="91028"/>
+                      <a14:foregroundMark x1="84595" y1="91028" x2="74224" y2="99148"/>
+                      <a14:foregroundMark x1="74224" y1="99148" x2="60220" y2="91028"/>
+                      <a14:foregroundMark x1="60220" y1="91028" x2="65140" y2="83986"/>
+                      <a14:foregroundMark x1="65140" y1="83986" x2="65140" y2="82169"/>
+                      <a14:foregroundMark x1="31643" y1="52016" x2="31643" y2="52470"/>
+                      <a14:foregroundMark x1="58554" y1="24248" x2="53936" y2="30721"/>
+                      <a14:foregroundMark x1="53936" y1="30721" x2="56851" y2="23169"/>
+                    </a14:backgroundRemoval>
+                  </a14:imgEffect>
+                </a14:imgLayer>
+              </a14:imgProps>
+            </a:ext>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2144486" y="1545772"/>
+          <a:ext cx="7772400" cy="5168315"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -539,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D625375-80E7-4819-8EFC-49100F2175E4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>